<commit_message>
Re-check for further understanding
</commit_message>
<xml_diff>
--- a/SE_FullFlex/testresult/testresult.xlsx
+++ b/SE_FullFlex/testresult/testresult.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\codekiemtra\CodecuaTien\SE_FullFlex\testresult\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\codekiemtra\SE_FullFlex\SE_FullFlex\testresult\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A2DD95D-9899-4A47-B312-6C7E7F50572D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E44DBE9D-80F0-4455-8079-C113210D8C19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{7DEC168E-F17A-4B8B-9EB7-E884DF0403C2}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="17">
   <si>
     <t>Test thử</t>
   </si>
@@ -84,12 +84,18 @@
   </si>
   <si>
     <t>1,3</t>
+  </si>
+  <si>
+    <t>Obj value</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.0000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -113,7 +119,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="7">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -157,41 +163,6 @@
         <color indexed="64"/>
       </right>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
       <bottom style="thin">
         <color indexed="64"/>
       </bottom>
@@ -201,7 +172,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -213,20 +184,26 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -235,32 +212,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Bình thường" xfId="0" builtinId="0"/>
@@ -595,10 +549,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{429A0A91-2162-4173-A323-1C3F7845F91F}">
-  <dimension ref="B1:L25"/>
+  <dimension ref="B1:S39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -608,31 +562,36 @@
     <col min="4" max="4" width="13" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B1" s="13" t="s">
+    <row r="1" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="14"/>
       <c r="D1" s="14"/>
       <c r="E1" s="14"/>
       <c r="F1" s="14"/>
-      <c r="G1" s="15"/>
-    </row>
-    <row r="2" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G1" s="14"/>
+      <c r="H1" s="14"/>
+    </row>
+    <row r="2" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="14" t="s">
         <v>7</v>
       </c>
-      <c r="E2" s="16"/>
-      <c r="F2" s="13" t="s">
+      <c r="E2" s="14"/>
+      <c r="F2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="G2" s="15"/>
-    </row>
-    <row r="3" spans="2:12" x14ac:dyDescent="0.2">
+      <c r="G2" s="14"/>
+      <c r="H2" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="2:19" x14ac:dyDescent="0.2">
       <c r="B3" s="2" t="s">
         <v>1</v>
       </c>
@@ -651,307 +610,669 @@
       <c r="G3" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I3" t="s">
+      <c r="H3" s="16"/>
+      <c r="J3" t="s">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>5</v>
       </c>
-      <c r="K3" t="s">
+      <c r="L3" t="s">
         <v>8</v>
       </c>
-      <c r="L3" t="s">
+      <c r="M3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="4" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B4" s="11">
-        <v>10</v>
+    <row r="4" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B4" s="14">
+        <v>5</v>
       </c>
       <c r="C4" s="1">
         <v>1</v>
       </c>
       <c r="D4" s="3">
-        <v>0.65369999999999995</v>
+        <v>0.113</v>
       </c>
       <c r="E4" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="F4" s="8">
-        <v>0.4</v>
-      </c>
-      <c r="G4" s="8"/>
-      <c r="K4" t="s">
+        <v>0.8</v>
+      </c>
+      <c r="F4" s="5">
+        <v>1</v>
+      </c>
+      <c r="G4" s="5"/>
+      <c r="H4" s="11">
+        <v>3.9979</v>
+      </c>
+      <c r="L4" t="s">
         <v>9</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="5" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B5" s="12"/>
+    <row r="5" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B5" s="14"/>
       <c r="C5" s="1">
         <v>3</v>
       </c>
       <c r="D5" s="3">
-        <v>11.5641</v>
+        <v>0.115</v>
       </c>
       <c r="E5" s="4">
-        <v>0.4</v>
-      </c>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="6" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B6" s="12"/>
+        <v>0.8</v>
+      </c>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+      <c r="H5" s="11">
+        <v>3.9981</v>
+      </c>
+    </row>
+    <row r="6" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B6" s="14"/>
       <c r="C6" s="1" t="s">
         <v>15</v>
       </c>
       <c r="D6" s="3">
-        <v>19.928999999999998</v>
+        <v>0.22800000000000001</v>
       </c>
       <c r="E6" s="4">
+        <v>1</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="G6" s="5">
+        <v>0.6</v>
+      </c>
+      <c r="H6" s="11">
+        <v>4.9973000000000001</v>
+      </c>
+    </row>
+    <row r="7" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="13"/>
+    </row>
+    <row r="8" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B8" s="14">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1">
+        <v>1</v>
+      </c>
+      <c r="D8" s="3">
+        <v>0.65</v>
+      </c>
+      <c r="E8" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="F8" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="G8" s="5"/>
+      <c r="H8" s="11">
+        <v>3.9984999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B9" s="14"/>
+      <c r="C9" s="1">
+        <v>3</v>
+      </c>
+      <c r="D9" s="3">
+        <v>11.56</v>
+      </c>
+      <c r="E9" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="H9" s="11">
+        <v>3.9981</v>
+      </c>
+      <c r="O9" s="6"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="8"/>
+      <c r="R9" s="9"/>
+      <c r="S9" s="9"/>
+    </row>
+    <row r="10" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B10" s="14"/>
+      <c r="C10" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D10" s="3">
+        <v>19.93</v>
+      </c>
+      <c r="E10" s="4">
         <v>0.5</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F10" s="5">
         <v>0.1</v>
       </c>
-      <c r="G6" s="8">
-        <v>0.4</v>
-      </c>
-    </row>
-    <row r="7" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B7" s="11">
+      <c r="G10" s="5">
+        <v>0.4</v>
+      </c>
+      <c r="H10" s="11">
+        <v>4.9972000000000003</v>
+      </c>
+      <c r="O10" s="6"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="8"/>
+      <c r="R10" s="9"/>
+      <c r="S10" s="9"/>
+    </row>
+    <row r="11" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B11" s="6"/>
+      <c r="C11" s="6"/>
+      <c r="D11" s="7"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="13"/>
+      <c r="O11" s="6"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="8"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+    </row>
+    <row r="12" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B12" s="14">
         <v>15</v>
       </c>
-      <c r="C7" s="1">
+      <c r="C12" s="1">
         <v>1</v>
       </c>
-      <c r="D7" s="3">
-        <v>0.84399999999999997</v>
-      </c>
-      <c r="E7" s="4">
-        <v>0.26600000000000001</v>
-      </c>
-      <c r="F7" s="8">
-        <v>0.26600000000000001</v>
-      </c>
-      <c r="G7" s="8"/>
-    </row>
-    <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="12"/>
-      <c r="C8" s="1">
+      <c r="D12" s="3">
+        <v>0.84</v>
+      </c>
+      <c r="E12" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="F12" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="G12" s="5"/>
+      <c r="H12" s="11">
+        <v>3.9984999999999999</v>
+      </c>
+      <c r="O12" s="6"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="8"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+    </row>
+    <row r="13" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B13" s="14"/>
+      <c r="C13" s="1">
         <v>3</v>
       </c>
-      <c r="D8" s="3">
-        <v>6.7370000000000001</v>
-      </c>
-      <c r="E8" s="4">
-        <v>0.2666</v>
-      </c>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8">
-        <v>0.26600000000000001</v>
-      </c>
-    </row>
-    <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="12"/>
-      <c r="C9" s="1" t="s">
+      <c r="D13" s="3">
+        <v>6.74</v>
+      </c>
+      <c r="E13" s="4">
+        <v>0.27</v>
+      </c>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5">
+        <v>0.27</v>
+      </c>
+      <c r="H13" s="11">
+        <v>3.9979</v>
+      </c>
+      <c r="O13" s="6"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="8"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+    </row>
+    <row r="14" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B14" s="14"/>
+      <c r="C14" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D14" s="3">
         <v>16.98</v>
       </c>
-      <c r="E9" s="4">
-        <v>0.2666</v>
-      </c>
-      <c r="F9" s="9">
-        <v>0.13300000000000001</v>
-      </c>
-      <c r="G9" s="8">
-        <v>0.6</v>
-      </c>
-    </row>
-    <row r="10" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B10" s="11">
+      <c r="E14" s="4">
+        <v>0.33300000000000002</v>
+      </c>
+      <c r="F14" s="5">
+        <v>0.13</v>
+      </c>
+      <c r="G14" s="5">
+        <v>0.2</v>
+      </c>
+      <c r="H14" s="11">
+        <v>4.9977</v>
+      </c>
+      <c r="O14" s="6"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="8"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+    </row>
+    <row r="15" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B15" s="6"/>
+      <c r="C15" s="6"/>
+      <c r="D15" s="7"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="13"/>
+      <c r="O15" s="6"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="8"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+    </row>
+    <row r="16" spans="2:19" x14ac:dyDescent="0.2">
+      <c r="B16" s="14">
         <v>20</v>
       </c>
-      <c r="C10" s="1">
+      <c r="C16" s="1">
         <v>1</v>
       </c>
-      <c r="D10" s="3">
-        <v>1.2452000000000001</v>
-      </c>
-      <c r="E10" s="4">
+      <c r="D16" s="10">
+        <v>1.25</v>
+      </c>
+      <c r="E16" s="4">
         <v>0.2</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F16" s="5">
         <v>0.2</v>
       </c>
-      <c r="G10" s="8"/>
-    </row>
-    <row r="11" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B11" s="12"/>
-      <c r="C11" s="1">
+      <c r="G16" s="2"/>
+      <c r="H16" s="11">
+        <v>3.9986000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="14"/>
+      <c r="C17" s="1">
         <v>3</v>
       </c>
-      <c r="D11" s="3">
-        <v>25.182500000000001</v>
-      </c>
-      <c r="E11" s="4">
+      <c r="D17" s="10">
+        <v>25.18</v>
+      </c>
+      <c r="E17" s="4">
         <v>0.2</v>
       </c>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8">
+      <c r="F17" s="2"/>
+      <c r="G17" s="5">
         <v>0.2</v>
       </c>
-    </row>
-    <row r="12" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B12" s="12"/>
-      <c r="C12" s="1" t="s">
+      <c r="H17" s="11">
+        <v>3.9981</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="14"/>
+      <c r="C18" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="3">
-        <v>22.208500000000001</v>
-      </c>
-      <c r="E12" s="4">
+      <c r="D18" s="10">
+        <v>22.21</v>
+      </c>
+      <c r="E18" s="4">
         <v>0.25</v>
       </c>
-      <c r="F12" s="8">
+      <c r="F18" s="5">
         <v>0.15</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G18" s="5">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="13" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B13" s="16">
-        <v>25</v>
-      </c>
-      <c r="C13" s="1">
+      <c r="H18" s="11">
+        <v>4.9973999999999998</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C19" s="6"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="9"/>
+      <c r="H19" s="13"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C20" s="6"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="8"/>
+      <c r="G20" s="9"/>
+      <c r="H20" s="13"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C21" s="6"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="13"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="G22" s="9"/>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="14">
+        <v>5</v>
+      </c>
+      <c r="C23" s="1">
         <v>1</v>
       </c>
-      <c r="D13" s="3">
-        <v>8.6501999999999999</v>
-      </c>
-      <c r="E13" s="4">
-        <v>0.16</v>
-      </c>
-      <c r="F13" s="8">
-        <v>0.16</v>
-      </c>
-      <c r="G13" s="8"/>
-    </row>
-    <row r="14" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B14" s="16"/>
-      <c r="C14" s="1">
+      <c r="D23" s="10">
+        <v>0.19</v>
+      </c>
+      <c r="E23" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="F23" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="G23" s="10"/>
+      <c r="H23" s="1">
+        <v>3.9973000000000001</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="14"/>
+      <c r="C24" s="1">
         <v>3</v>
       </c>
-      <c r="D14" s="3">
-        <v>3.6936</v>
-      </c>
-      <c r="E14" s="4">
-        <v>0.16</v>
-      </c>
-      <c r="F14" s="8">
-        <v>0.16</v>
-      </c>
-      <c r="G14" s="8"/>
-    </row>
-    <row r="15" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B15" s="16"/>
-      <c r="C15" s="1" t="s">
+      <c r="D24" s="10">
+        <v>2.57</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="F24" s="10"/>
+      <c r="G24" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="H24" s="1">
+        <v>3.9971999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="14"/>
+      <c r="C25" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="3">
-        <v>109.209</v>
-      </c>
-      <c r="E15" s="4">
+      <c r="D25" s="10">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="E25" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="F25" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="G25" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="H25" s="1">
+        <v>3.9969999999999999</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C26" s="6"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="12"/>
+      <c r="H26" s="6"/>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B27" s="14">
+        <v>8</v>
+      </c>
+      <c r="C27" s="1">
+        <v>1</v>
+      </c>
+      <c r="D27" s="10">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="E27" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F27" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="G27" s="10"/>
+      <c r="H27" s="1">
+        <v>3.9954999999999998</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B28" s="14"/>
+      <c r="C28" s="1">
+        <v>3</v>
+      </c>
+      <c r="D28" s="10">
+        <v>1.44</v>
+      </c>
+      <c r="E28" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F28" s="10"/>
+      <c r="G28" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="H28" s="1">
+        <v>3.9971000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B29" s="14"/>
+      <c r="C29" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="10">
+        <v>0.68</v>
+      </c>
+      <c r="E29" s="10">
+        <v>0.5</v>
+      </c>
+      <c r="F29" s="10">
+        <v>0.375</v>
+      </c>
+      <c r="G29" s="10">
+        <v>0.125</v>
+      </c>
+      <c r="H29" s="1">
+        <v>3.9975000000000001</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="C30" s="6"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="12"/>
+      <c r="F30" s="12"/>
+      <c r="G30" s="12"/>
+      <c r="H30" s="6"/>
+    </row>
+    <row r="31" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B31" s="14">
+        <v>10</v>
+      </c>
+      <c r="C31" s="1">
+        <v>1</v>
+      </c>
+      <c r="D31" s="10">
+        <v>0.24</v>
+      </c>
+      <c r="E31" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="F31" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="G31" s="10"/>
+      <c r="H31" s="1">
+        <v>3.9961000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B32" s="14"/>
+      <c r="C32" s="1">
+        <v>3</v>
+      </c>
+      <c r="D32" s="10">
+        <v>1.53</v>
+      </c>
+      <c r="E32" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="F32" s="10"/>
+      <c r="G32" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="H32" s="1">
+        <v>3.9971999999999999</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B33" s="14"/>
+      <c r="C33" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="10">
+        <v>0.31</v>
+      </c>
+      <c r="E33" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="F33" s="10">
+        <v>0.4</v>
+      </c>
+      <c r="G33" s="10"/>
+      <c r="H33" s="1">
+        <v>3.9962</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="14" t="s">
+        <v>7</v>
+      </c>
+      <c r="E35" s="14"/>
+      <c r="F35" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="G35" s="14"/>
+      <c r="H35" s="15" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B36" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D36" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E36" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="H36" s="16"/>
+    </row>
+    <row r="37" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B37" s="14">
+        <v>15</v>
+      </c>
+      <c r="C37" s="1">
+        <v>1</v>
+      </c>
+      <c r="D37" s="10">
+        <v>4.6242999999999999</v>
+      </c>
+      <c r="E37" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="F37" s="10">
+        <v>0.8</v>
+      </c>
+      <c r="G37" s="10"/>
+      <c r="H37" s="17">
+        <v>11.53</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B38" s="14"/>
+      <c r="C38" s="1">
+        <v>3</v>
+      </c>
+      <c r="D38" s="10">
+        <v>333.56939999999997</v>
+      </c>
+      <c r="E38" s="10">
+        <v>0.93330000000000002</v>
+      </c>
+      <c r="F38" s="10"/>
+      <c r="G38" s="10">
+        <v>0.93332999999999999</v>
+      </c>
+      <c r="H38" s="17">
+        <v>13.31</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B39" s="14"/>
+      <c r="C39" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="10">
+        <v>468.9735</v>
+      </c>
+      <c r="E39" s="10">
+        <v>0.93330000000000002</v>
+      </c>
+      <c r="F39" s="10">
         <v>0.2</v>
       </c>
-      <c r="F15" s="8">
-        <v>0.12</v>
-      </c>
-      <c r="G15" s="8">
-        <v>0.08</v>
-      </c>
-    </row>
-    <row r="16" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B16" s="17"/>
-      <c r="C16" s="18"/>
-      <c r="D16" s="19"/>
-      <c r="E16" s="20"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-    </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B17" s="17"/>
-      <c r="C17" s="18"/>
-      <c r="D17" s="19"/>
-      <c r="E17" s="20"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-    </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B18" s="17"/>
-      <c r="C18" s="18"/>
-      <c r="D18" s="19"/>
-      <c r="E18" s="20"/>
-      <c r="F18" s="22"/>
-      <c r="G18" s="22"/>
-    </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B19" s="17"/>
-      <c r="C19" s="18"/>
-      <c r="D19" s="19"/>
-      <c r="E19" s="20"/>
-      <c r="F19" s="22"/>
-      <c r="G19" s="22"/>
-    </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B20" s="10"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="7"/>
-      <c r="E20" s="6"/>
-    </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="B21" s="10"/>
-      <c r="C21" s="5"/>
-      <c r="D21" s="7"/>
-      <c r="E21" s="6"/>
-    </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C22" s="5"/>
-      <c r="D22" s="7"/>
-      <c r="E22" s="6"/>
-    </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C23" s="5"/>
-      <c r="D23" s="7"/>
-      <c r="E23" s="6"/>
-    </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C24" s="5"/>
-      <c r="D24" s="7"/>
-      <c r="E24" s="6"/>
-    </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.2">
-      <c r="C25" s="5"/>
-      <c r="D25" s="7"/>
-      <c r="E25" s="6"/>
+      <c r="G39" s="10">
+        <v>0.73333000000000004</v>
+      </c>
+      <c r="H39" s="17">
+        <v>13.35</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="B1:G1"/>
+  <mergeCells count="15">
+    <mergeCell ref="B37:B39"/>
+    <mergeCell ref="D35:E35"/>
+    <mergeCell ref="F35:G35"/>
+    <mergeCell ref="H35:H36"/>
+    <mergeCell ref="B23:B25"/>
+    <mergeCell ref="B27:B29"/>
+    <mergeCell ref="B31:B33"/>
+    <mergeCell ref="B12:B14"/>
+    <mergeCell ref="B1:H1"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="H2:H3"/>
     <mergeCell ref="D2:E2"/>
     <mergeCell ref="B4:B6"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B8:B10"/>
     <mergeCell ref="F2:G2"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>